<commit_message>
Spreadsheet with limited data, only the variables we need
</commit_message>
<xml_diff>
--- a/B3_102_limdata.xlsx
+++ b/B3_102_limdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yujia1998/Desktop/Work/Reading Center/B3VF/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC4EAC5-16E1-284D-8BED-753A334BD2F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A7C60D-0053-9841-8385-DAED1CF3AE1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28800" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -933,6 +933,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1410,10 +1413,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1771,13 +1775,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C414C91-2AD7-EA4E-96F3-D5F16D2BDCF8}">
   <dimension ref="A1:I252"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1791,7 +1795,7 @@
       <c r="C1" t="s">
         <v>300</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>298</v>
       </c>
       <c r="E1" t="s">
@@ -1820,7 +1824,7 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="3">
         <v>44999</v>
       </c>
       <c r="E2" t="s">
@@ -1849,7 +1853,7 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="3">
         <v>44999</v>
       </c>
       <c r="E3" t="s">
@@ -1878,7 +1882,7 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="3">
         <v>44999</v>
       </c>
       <c r="E4" t="s">
@@ -1907,7 +1911,7 @@
       <c r="C5">
         <v>2</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="3">
         <v>45090</v>
       </c>
       <c r="E5" t="s">
@@ -1936,7 +1940,7 @@
       <c r="C6">
         <v>2</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="3">
         <v>45090</v>
       </c>
       <c r="E6" t="s">
@@ -1965,7 +1969,7 @@
       <c r="C7">
         <v>2</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="3">
         <v>45090</v>
       </c>
       <c r="E7" t="s">
@@ -1994,7 +1998,7 @@
       <c r="C8">
         <v>1</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="3">
         <v>45012</v>
       </c>
       <c r="E8" t="s">
@@ -2023,7 +2027,7 @@
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="3">
         <v>45012</v>
       </c>
       <c r="E9" t="s">
@@ -2052,7 +2056,7 @@
       <c r="C10">
         <v>1</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="3">
         <v>45012</v>
       </c>
       <c r="E10" t="s">
@@ -2081,7 +2085,7 @@
       <c r="C11">
         <v>2</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="3">
         <v>45084</v>
       </c>
       <c r="E11" t="s">
@@ -2110,7 +2114,7 @@
       <c r="C12">
         <v>2</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="3">
         <v>45084</v>
       </c>
       <c r="E12" t="s">
@@ -2139,7 +2143,7 @@
       <c r="C13">
         <v>1</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="3">
         <v>45015</v>
       </c>
       <c r="E13" t="s">
@@ -2168,7 +2172,7 @@
       <c r="C14">
         <v>1</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="3">
         <v>45015</v>
       </c>
       <c r="E14" t="s">
@@ -2197,7 +2201,7 @@
       <c r="C15">
         <v>1</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="3">
         <v>45015</v>
       </c>
       <c r="E15" t="s">
@@ -2226,7 +2230,7 @@
       <c r="C16">
         <v>2</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="3">
         <v>45086</v>
       </c>
       <c r="E16" t="s">
@@ -2255,7 +2259,7 @@
       <c r="C17">
         <v>2</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="3">
         <v>45086</v>
       </c>
       <c r="E17" t="s">
@@ -2284,7 +2288,7 @@
       <c r="C18">
         <v>1</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="3">
         <v>45020</v>
       </c>
       <c r="E18" t="s">
@@ -2313,7 +2317,7 @@
       <c r="C19">
         <v>1</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="3">
         <v>45020</v>
       </c>
       <c r="E19" t="s">
@@ -2342,7 +2346,7 @@
       <c r="C20">
         <v>1</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="3">
         <v>45020</v>
       </c>
       <c r="E20" t="s">
@@ -2371,7 +2375,7 @@
       <c r="C21">
         <v>2</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="3">
         <v>45097</v>
       </c>
       <c r="E21" t="s">
@@ -2400,7 +2404,7 @@
       <c r="C22">
         <v>2</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="3">
         <v>45097</v>
       </c>
       <c r="E22" t="s">
@@ -2429,7 +2433,7 @@
       <c r="C23">
         <v>2</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23" s="3">
         <v>45097</v>
       </c>
       <c r="E23" t="s">
@@ -2458,7 +2462,7 @@
       <c r="C24">
         <v>1</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24" s="3">
         <v>45027</v>
       </c>
       <c r="E24" t="s">
@@ -2487,7 +2491,7 @@
       <c r="C25">
         <v>1</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25" s="3">
         <v>45048</v>
       </c>
       <c r="E25" t="s">
@@ -2516,7 +2520,7 @@
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26" s="3">
         <v>45048</v>
       </c>
       <c r="E26" t="s">
@@ -2545,7 +2549,7 @@
       <c r="C27">
         <v>2</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27" s="3">
         <v>45118</v>
       </c>
       <c r="E27" t="s">
@@ -2574,7 +2578,7 @@
       <c r="C28">
         <v>2</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28" s="3">
         <v>45118</v>
       </c>
       <c r="E28" t="s">
@@ -2603,7 +2607,7 @@
       <c r="C29">
         <v>2</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29" s="3">
         <v>45118</v>
       </c>
       <c r="E29" t="s">
@@ -2629,7 +2633,10 @@
       <c r="B30" t="s">
         <v>11</v>
       </c>
-      <c r="D30" s="1">
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30" s="3">
         <v>45027</v>
       </c>
       <c r="E30" t="s">
@@ -2655,7 +2662,10 @@
       <c r="B31" t="s">
         <v>11</v>
       </c>
-      <c r="D31" s="1">
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31" s="3">
         <v>45033</v>
       </c>
       <c r="E31" t="s">
@@ -2681,7 +2691,10 @@
       <c r="B32" t="s">
         <v>11</v>
       </c>
-      <c r="D32" s="1">
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" s="3">
         <v>45033</v>
       </c>
       <c r="E32" t="s">
@@ -2707,7 +2720,10 @@
       <c r="B33" t="s">
         <v>11</v>
       </c>
-      <c r="D33" s="1">
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33" s="3">
         <v>45107</v>
       </c>
       <c r="E33" t="s">
@@ -2733,7 +2749,10 @@
       <c r="B34" t="s">
         <v>11</v>
       </c>
-      <c r="D34" s="1">
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34" s="3">
         <v>45107</v>
       </c>
       <c r="E34" t="s">
@@ -2759,7 +2778,10 @@
       <c r="B35" t="s">
         <v>11</v>
       </c>
-      <c r="D35" s="1">
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35" s="3">
         <v>45107</v>
       </c>
       <c r="E35" t="s">
@@ -2785,7 +2807,10 @@
       <c r="B36" t="s">
         <v>6</v>
       </c>
-      <c r="D36" s="1">
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36" s="3">
         <v>45029</v>
       </c>
       <c r="E36" t="s">
@@ -2811,7 +2836,10 @@
       <c r="B37" t="s">
         <v>6</v>
       </c>
-      <c r="D37" s="1">
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37" s="3">
         <v>45029</v>
       </c>
       <c r="E37" t="s">
@@ -2837,7 +2865,10 @@
       <c r="B38" t="s">
         <v>6</v>
       </c>
-      <c r="D38" s="1">
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38" s="3">
         <v>45029</v>
       </c>
       <c r="E38" t="s">
@@ -2863,7 +2894,10 @@
       <c r="B39" t="s">
         <v>6</v>
       </c>
-      <c r="D39" s="1">
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="D39" s="3">
         <v>45091</v>
       </c>
       <c r="E39" t="s">
@@ -2889,7 +2923,10 @@
       <c r="B40" t="s">
         <v>6</v>
       </c>
-      <c r="D40" s="1">
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40" s="3">
         <v>45091</v>
       </c>
       <c r="E40" t="s">
@@ -2915,7 +2952,10 @@
       <c r="B41" t="s">
         <v>6</v>
       </c>
-      <c r="D41" s="1">
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41" s="3">
         <v>45091</v>
       </c>
       <c r="E41" t="s">
@@ -2941,7 +2981,7 @@
       <c r="B42" t="s">
         <v>11</v>
       </c>
-      <c r="D42" s="1">
+      <c r="D42" s="3">
         <v>45033</v>
       </c>
       <c r="E42" t="s">
@@ -2967,7 +3007,7 @@
       <c r="B43" t="s">
         <v>11</v>
       </c>
-      <c r="D43" s="1">
+      <c r="D43" s="3">
         <v>45033</v>
       </c>
       <c r="E43" t="s">
@@ -2993,7 +3033,7 @@
       <c r="B44" t="s">
         <v>11</v>
       </c>
-      <c r="D44" s="1">
+      <c r="D44" s="3">
         <v>45033</v>
       </c>
       <c r="E44" t="s">
@@ -3019,7 +3059,7 @@
       <c r="B45" t="s">
         <v>11</v>
       </c>
-      <c r="D45" s="1">
+      <c r="D45" s="3">
         <v>45103</v>
       </c>
       <c r="E45" t="s">
@@ -3045,7 +3085,7 @@
       <c r="B46" t="s">
         <v>11</v>
       </c>
-      <c r="D46" s="1">
+      <c r="D46" s="3">
         <v>45103</v>
       </c>
       <c r="E46" t="s">
@@ -3071,7 +3111,7 @@
       <c r="B47" t="s">
         <v>11</v>
       </c>
-      <c r="D47" s="1">
+      <c r="D47" s="3">
         <v>45103</v>
       </c>
       <c r="E47" t="s">
@@ -3097,7 +3137,7 @@
       <c r="B48" t="s">
         <v>11</v>
       </c>
-      <c r="D48" s="1">
+      <c r="D48" s="3">
         <v>45035</v>
       </c>
       <c r="E48" t="s">
@@ -3123,7 +3163,7 @@
       <c r="B49" t="s">
         <v>11</v>
       </c>
-      <c r="D49" s="1">
+      <c r="D49" s="3">
         <v>45035</v>
       </c>
       <c r="E49" t="s">
@@ -3149,7 +3189,7 @@
       <c r="B50" t="s">
         <v>11</v>
       </c>
-      <c r="D50" s="1">
+      <c r="D50" s="3">
         <v>45035</v>
       </c>
       <c r="E50" t="s">
@@ -3175,7 +3215,7 @@
       <c r="B51" t="s">
         <v>11</v>
       </c>
-      <c r="D51" s="1">
+      <c r="D51" s="3">
         <v>45119</v>
       </c>
       <c r="E51" t="s">
@@ -3201,7 +3241,7 @@
       <c r="B52" t="s">
         <v>11</v>
       </c>
-      <c r="D52" s="1">
+      <c r="D52" s="3">
         <v>45119</v>
       </c>
       <c r="E52" t="s">
@@ -3227,7 +3267,7 @@
       <c r="B53" t="s">
         <v>11</v>
       </c>
-      <c r="D53" s="1">
+      <c r="D53" s="3">
         <v>45119</v>
       </c>
       <c r="E53" t="s">
@@ -3253,7 +3293,7 @@
       <c r="B54" t="s">
         <v>6</v>
       </c>
-      <c r="D54" s="1">
+      <c r="D54" s="3">
         <v>45036</v>
       </c>
       <c r="E54" s="2">
@@ -3279,7 +3319,7 @@
       <c r="B55" t="s">
         <v>6</v>
       </c>
-      <c r="D55" s="1">
+      <c r="D55" s="3">
         <v>45036</v>
       </c>
       <c r="E55" s="2">
@@ -3305,7 +3345,7 @@
       <c r="B56" t="s">
         <v>6</v>
       </c>
-      <c r="D56" s="1">
+      <c r="D56" s="3">
         <v>45036</v>
       </c>
       <c r="E56" s="2">
@@ -3331,7 +3371,7 @@
       <c r="B57" t="s">
         <v>11</v>
       </c>
-      <c r="D57" s="1">
+      <c r="D57" s="3">
         <v>45037</v>
       </c>
       <c r="E57" t="s">
@@ -3357,7 +3397,7 @@
       <c r="B58" t="s">
         <v>11</v>
       </c>
-      <c r="D58" s="1">
+      <c r="D58" s="3">
         <v>45037</v>
       </c>
       <c r="E58" t="s">
@@ -3383,7 +3423,7 @@
       <c r="B59" t="s">
         <v>11</v>
       </c>
-      <c r="D59" s="1">
+      <c r="D59" s="3">
         <v>45037</v>
       </c>
       <c r="E59" t="s">
@@ -3409,7 +3449,7 @@
       <c r="B60" t="s">
         <v>11</v>
       </c>
-      <c r="D60" s="1">
+      <c r="D60" s="3">
         <v>45121</v>
       </c>
       <c r="E60" s="2">
@@ -3435,7 +3475,7 @@
       <c r="B61" t="s">
         <v>11</v>
       </c>
-      <c r="D61" s="1">
+      <c r="D61" s="3">
         <v>45121</v>
       </c>
       <c r="E61" t="s">
@@ -3461,7 +3501,7 @@
       <c r="B62" t="s">
         <v>11</v>
       </c>
-      <c r="D62" s="1">
+      <c r="D62" s="3">
         <v>45121</v>
       </c>
       <c r="E62" t="s">
@@ -3487,7 +3527,7 @@
       <c r="B63" t="s">
         <v>11</v>
       </c>
-      <c r="D63" s="1">
+      <c r="D63" s="3">
         <v>45040</v>
       </c>
       <c r="E63" t="s">
@@ -3513,7 +3553,7 @@
       <c r="B64" t="s">
         <v>11</v>
       </c>
-      <c r="D64" s="1">
+      <c r="D64" s="3">
         <v>45040</v>
       </c>
       <c r="E64" t="s">
@@ -3539,7 +3579,7 @@
       <c r="B65" t="s">
         <v>11</v>
       </c>
-      <c r="D65" s="1">
+      <c r="D65" s="3">
         <v>45126</v>
       </c>
       <c r="E65" t="s">
@@ -3565,7 +3605,7 @@
       <c r="B66" t="s">
         <v>11</v>
       </c>
-      <c r="D66" s="1">
+      <c r="D66" s="3">
         <v>45126</v>
       </c>
       <c r="E66" t="s">
@@ -3591,7 +3631,7 @@
       <c r="B67" t="s">
         <v>11</v>
       </c>
-      <c r="D67" s="1">
+      <c r="D67" s="3">
         <v>45126</v>
       </c>
       <c r="E67" t="s">
@@ -3617,7 +3657,7 @@
       <c r="B68" t="s">
         <v>6</v>
       </c>
-      <c r="D68" s="1">
+      <c r="D68" s="3">
         <v>45040</v>
       </c>
       <c r="E68" t="s">
@@ -3643,7 +3683,7 @@
       <c r="B69" t="s">
         <v>6</v>
       </c>
-      <c r="D69" s="1">
+      <c r="D69" s="3">
         <v>45040</v>
       </c>
       <c r="E69" t="s">
@@ -3669,7 +3709,7 @@
       <c r="B70" t="s">
         <v>6</v>
       </c>
-      <c r="D70" s="1">
+      <c r="D70" s="3">
         <v>45040</v>
       </c>
       <c r="E70" t="s">
@@ -3695,7 +3735,7 @@
       <c r="B71" t="s">
         <v>6</v>
       </c>
-      <c r="D71" s="1">
+      <c r="D71" s="3">
         <v>45124</v>
       </c>
       <c r="E71" t="s">
@@ -3721,7 +3761,7 @@
       <c r="B72" t="s">
         <v>6</v>
       </c>
-      <c r="D72" s="1">
+      <c r="D72" s="3">
         <v>45124</v>
       </c>
       <c r="E72" t="s">
@@ -3747,7 +3787,7 @@
       <c r="B73" t="s">
         <v>6</v>
       </c>
-      <c r="D73" s="1">
+      <c r="D73" s="3">
         <v>45124</v>
       </c>
       <c r="E73" t="s">
@@ -3773,7 +3813,7 @@
       <c r="B74" t="s">
         <v>11</v>
       </c>
-      <c r="D74" s="1">
+      <c r="D74" s="3">
         <v>45048</v>
       </c>
       <c r="E74" t="s">
@@ -3799,7 +3839,7 @@
       <c r="B75" t="s">
         <v>11</v>
       </c>
-      <c r="D75" s="1">
+      <c r="D75" s="3">
         <v>45048</v>
       </c>
       <c r="E75" t="s">
@@ -3825,7 +3865,7 @@
       <c r="B76" t="s">
         <v>11</v>
       </c>
-      <c r="D76" s="1">
+      <c r="D76" s="3">
         <v>45048</v>
       </c>
       <c r="E76" t="s">
@@ -3851,7 +3891,7 @@
       <c r="B77" t="s">
         <v>11</v>
       </c>
-      <c r="D77" s="1">
+      <c r="D77" s="3">
         <v>45132</v>
       </c>
       <c r="E77" t="s">
@@ -3877,7 +3917,7 @@
       <c r="B78" t="s">
         <v>11</v>
       </c>
-      <c r="D78" s="1">
+      <c r="D78" s="3">
         <v>45132</v>
       </c>
       <c r="E78" t="s">
@@ -3903,7 +3943,7 @@
       <c r="B79" t="s">
         <v>11</v>
       </c>
-      <c r="D79" s="1">
+      <c r="D79" s="3">
         <v>45132</v>
       </c>
       <c r="E79" t="s">
@@ -3929,7 +3969,7 @@
       <c r="B80" t="s">
         <v>11</v>
       </c>
-      <c r="D80" s="1">
+      <c r="D80" s="3">
         <v>45070</v>
       </c>
       <c r="E80" t="s">
@@ -3955,7 +3995,7 @@
       <c r="B81" t="s">
         <v>11</v>
       </c>
-      <c r="D81" s="1">
+      <c r="D81" s="3">
         <v>45070</v>
       </c>
       <c r="E81" t="s">
@@ -3981,7 +4021,7 @@
       <c r="B82" t="s">
         <v>11</v>
       </c>
-      <c r="D82" s="1">
+      <c r="D82" s="3">
         <v>45070</v>
       </c>
       <c r="E82" t="s">
@@ -4007,7 +4047,7 @@
       <c r="B83" t="s">
         <v>11</v>
       </c>
-      <c r="D83" s="1">
+      <c r="D83" s="3">
         <v>45126</v>
       </c>
       <c r="E83" t="s">
@@ -4033,7 +4073,7 @@
       <c r="B84" t="s">
         <v>11</v>
       </c>
-      <c r="D84" s="1">
+      <c r="D84" s="3">
         <v>45126</v>
       </c>
       <c r="E84" t="s">
@@ -4059,7 +4099,7 @@
       <c r="B85" t="s">
         <v>11</v>
       </c>
-      <c r="D85" s="1">
+      <c r="D85" s="3">
         <v>45042</v>
       </c>
       <c r="E85" s="2">
@@ -4085,7 +4125,7 @@
       <c r="B86" t="s">
         <v>11</v>
       </c>
-      <c r="D86" s="1">
+      <c r="D86" s="3">
         <v>45042</v>
       </c>
       <c r="E86" s="2">
@@ -4111,7 +4151,7 @@
       <c r="B87" t="s">
         <v>11</v>
       </c>
-      <c r="D87" s="1">
+      <c r="D87" s="3">
         <v>45042</v>
       </c>
       <c r="E87" s="2">
@@ -4137,7 +4177,7 @@
       <c r="B88" t="s">
         <v>11</v>
       </c>
-      <c r="D88" s="1">
+      <c r="D88" s="3">
         <v>45103</v>
       </c>
       <c r="E88" s="2">
@@ -4163,7 +4203,7 @@
       <c r="B89" t="s">
         <v>11</v>
       </c>
-      <c r="D89" s="1">
+      <c r="D89" s="3">
         <v>45103</v>
       </c>
       <c r="E89" s="2">
@@ -4189,7 +4229,7 @@
       <c r="B90" t="s">
         <v>11</v>
       </c>
-      <c r="D90" s="1">
+      <c r="D90" s="3">
         <v>45103</v>
       </c>
       <c r="E90" s="2">
@@ -4215,7 +4255,7 @@
       <c r="B91" t="s">
         <v>6</v>
       </c>
-      <c r="D91" s="1">
+      <c r="D91" s="3">
         <v>45042</v>
       </c>
       <c r="E91" t="s">
@@ -4241,7 +4281,7 @@
       <c r="B92" t="s">
         <v>6</v>
       </c>
-      <c r="D92" s="1">
+      <c r="D92" s="3">
         <v>45042</v>
       </c>
       <c r="E92" t="s">
@@ -4267,7 +4307,7 @@
       <c r="B93" t="s">
         <v>6</v>
       </c>
-      <c r="D93" s="1">
+      <c r="D93" s="3">
         <v>45042</v>
       </c>
       <c r="E93" t="s">
@@ -4293,7 +4333,7 @@
       <c r="B94" t="s">
         <v>11</v>
       </c>
-      <c r="D94" s="1">
+      <c r="D94" s="3">
         <v>45044</v>
       </c>
       <c r="E94" t="s">
@@ -4319,7 +4359,7 @@
       <c r="B95" t="s">
         <v>11</v>
       </c>
-      <c r="D95" s="1">
+      <c r="D95" s="3">
         <v>45044</v>
       </c>
       <c r="E95" t="s">
@@ -4345,7 +4385,7 @@
       <c r="B96" t="s">
         <v>11</v>
       </c>
-      <c r="D96" s="1">
+      <c r="D96" s="3">
         <v>45044</v>
       </c>
       <c r="E96" t="s">
@@ -4371,7 +4411,7 @@
       <c r="B97" t="s">
         <v>6</v>
       </c>
-      <c r="D97" s="1">
+      <c r="D97" s="3">
         <v>45047</v>
       </c>
       <c r="E97" t="s">
@@ -4397,7 +4437,7 @@
       <c r="B98" t="s">
         <v>6</v>
       </c>
-      <c r="D98" s="1">
+      <c r="D98" s="3">
         <v>45047</v>
       </c>
       <c r="E98" t="s">
@@ -4423,7 +4463,7 @@
       <c r="B99" t="s">
         <v>6</v>
       </c>
-      <c r="D99" s="1">
+      <c r="D99" s="3">
         <v>45047</v>
       </c>
       <c r="E99" t="s">
@@ -4449,7 +4489,7 @@
       <c r="B100" t="s">
         <v>6</v>
       </c>
-      <c r="D100" s="1">
+      <c r="D100" s="3">
         <v>45124</v>
       </c>
       <c r="E100" t="s">
@@ -4475,7 +4515,7 @@
       <c r="B101" t="s">
         <v>6</v>
       </c>
-      <c r="D101" s="1">
+      <c r="D101" s="3">
         <v>45124</v>
       </c>
       <c r="E101" t="s">
@@ -4501,7 +4541,7 @@
       <c r="B102" t="s">
         <v>6</v>
       </c>
-      <c r="D102" s="1">
+      <c r="D102" s="3">
         <v>45124</v>
       </c>
       <c r="E102" t="s">
@@ -4527,7 +4567,7 @@
       <c r="B103" t="s">
         <v>11</v>
       </c>
-      <c r="D103" s="1">
+      <c r="D103" s="3">
         <v>45047</v>
       </c>
       <c r="E103" t="s">
@@ -4553,7 +4593,7 @@
       <c r="B104" t="s">
         <v>11</v>
       </c>
-      <c r="D104" s="1">
+      <c r="D104" s="3">
         <v>45047</v>
       </c>
       <c r="E104" t="s">
@@ -4579,7 +4619,7 @@
       <c r="B105" t="s">
         <v>11</v>
       </c>
-      <c r="D105" s="1">
+      <c r="D105" s="3">
         <v>45047</v>
       </c>
       <c r="E105" t="s">
@@ -4605,7 +4645,7 @@
       <c r="B106" t="s">
         <v>11</v>
       </c>
-      <c r="D106" s="1">
+      <c r="D106" s="3">
         <v>45117</v>
       </c>
       <c r="E106" t="s">
@@ -4631,7 +4671,7 @@
       <c r="B107" t="s">
         <v>11</v>
       </c>
-      <c r="D107" s="1">
+      <c r="D107" s="3">
         <v>45117</v>
       </c>
       <c r="E107" t="s">
@@ -4657,7 +4697,7 @@
       <c r="B108" t="s">
         <v>11</v>
       </c>
-      <c r="D108" s="1">
+      <c r="D108" s="3">
         <v>45117</v>
       </c>
       <c r="E108" t="s">
@@ -4683,7 +4723,7 @@
       <c r="B109" t="s">
         <v>6</v>
       </c>
-      <c r="D109" s="1">
+      <c r="D109" s="3">
         <v>45049</v>
       </c>
       <c r="E109" t="s">
@@ -4709,7 +4749,7 @@
       <c r="B110" t="s">
         <v>6</v>
       </c>
-      <c r="D110" s="1">
+      <c r="D110" s="3">
         <v>45049</v>
       </c>
       <c r="E110" t="s">
@@ -4735,7 +4775,7 @@
       <c r="B111" t="s">
         <v>6</v>
       </c>
-      <c r="D111" s="1">
+      <c r="D111" s="3">
         <v>45049</v>
       </c>
       <c r="E111" t="s">
@@ -4761,7 +4801,7 @@
       <c r="B112" t="s">
         <v>6</v>
       </c>
-      <c r="D112" s="1">
+      <c r="D112" s="3">
         <v>45120</v>
       </c>
       <c r="E112" t="s">
@@ -4787,7 +4827,7 @@
       <c r="B113" t="s">
         <v>6</v>
       </c>
-      <c r="D113" s="1">
+      <c r="D113" s="3">
         <v>45120</v>
       </c>
       <c r="E113" t="s">
@@ -4813,7 +4853,7 @@
       <c r="B114" t="s">
         <v>6</v>
       </c>
-      <c r="D114" s="1">
+      <c r="D114" s="3">
         <v>45120</v>
       </c>
       <c r="E114" t="s">
@@ -4839,7 +4879,7 @@
       <c r="B115" t="s">
         <v>6</v>
       </c>
-      <c r="D115" s="1">
+      <c r="D115" s="3">
         <v>45037</v>
       </c>
       <c r="E115" t="s">
@@ -4865,7 +4905,7 @@
       <c r="B116" t="s">
         <v>6</v>
       </c>
-      <c r="D116" s="1">
+      <c r="D116" s="3">
         <v>45051</v>
       </c>
       <c r="E116" t="s">
@@ -4891,7 +4931,7 @@
       <c r="B117" t="s">
         <v>6</v>
       </c>
-      <c r="D117" s="1">
+      <c r="D117" s="3">
         <v>45051</v>
       </c>
       <c r="E117" t="s">
@@ -4917,7 +4957,7 @@
       <c r="B118" t="s">
         <v>6</v>
       </c>
-      <c r="D118" s="1">
+      <c r="D118" s="3">
         <v>45100</v>
       </c>
       <c r="E118" s="2">
@@ -4943,7 +4983,7 @@
       <c r="B119" t="s">
         <v>6</v>
       </c>
-      <c r="D119" s="1">
+      <c r="D119" s="3">
         <v>45100</v>
       </c>
       <c r="E119" s="2">
@@ -4969,7 +5009,7 @@
       <c r="B120" t="s">
         <v>6</v>
       </c>
-      <c r="D120" s="1">
+      <c r="D120" s="3">
         <v>45100</v>
       </c>
       <c r="E120" t="s">
@@ -4995,7 +5035,7 @@
       <c r="B121" t="s">
         <v>6</v>
       </c>
-      <c r="D121" s="1">
+      <c r="D121" s="3">
         <v>45139</v>
       </c>
       <c r="E121" t="s">
@@ -5021,7 +5061,7 @@
       <c r="B122" t="s">
         <v>6</v>
       </c>
-      <c r="D122" s="1">
+      <c r="D122" s="3">
         <v>45139</v>
       </c>
       <c r="E122" t="s">
@@ -5047,7 +5087,7 @@
       <c r="B123" t="s">
         <v>6</v>
       </c>
-      <c r="D123" s="1">
+      <c r="D123" s="3">
         <v>45145</v>
       </c>
       <c r="E123" t="s">
@@ -5073,7 +5113,7 @@
       <c r="B124" t="s">
         <v>11</v>
       </c>
-      <c r="D124" s="1">
+      <c r="D124" s="3">
         <v>45054</v>
       </c>
       <c r="E124" t="s">
@@ -5099,7 +5139,7 @@
       <c r="B125" t="s">
         <v>11</v>
       </c>
-      <c r="D125" s="1">
+      <c r="D125" s="3">
         <v>45054</v>
       </c>
       <c r="E125" t="s">
@@ -5125,7 +5165,7 @@
       <c r="B126" t="s">
         <v>11</v>
       </c>
-      <c r="D126" s="1">
+      <c r="D126" s="3">
         <v>45054</v>
       </c>
       <c r="E126" t="s">
@@ -5151,7 +5191,7 @@
       <c r="B127" t="s">
         <v>11</v>
       </c>
-      <c r="D127" s="1">
+      <c r="D127" s="3">
         <v>45124</v>
       </c>
       <c r="E127" t="s">
@@ -5177,7 +5217,7 @@
       <c r="B128" t="s">
         <v>11</v>
       </c>
-      <c r="D128" s="1">
+      <c r="D128" s="3">
         <v>45124</v>
       </c>
       <c r="E128" t="s">
@@ -5203,7 +5243,7 @@
       <c r="B129" t="s">
         <v>11</v>
       </c>
-      <c r="D129" s="1">
+      <c r="D129" s="3">
         <v>45124</v>
       </c>
       <c r="E129" t="s">
@@ -5229,7 +5269,7 @@
       <c r="B130" t="s">
         <v>11</v>
       </c>
-      <c r="D130" s="1">
+      <c r="D130" s="3">
         <v>45058</v>
       </c>
       <c r="E130" t="s">
@@ -5255,7 +5295,7 @@
       <c r="B131" t="s">
         <v>11</v>
       </c>
-      <c r="D131" s="1">
+      <c r="D131" s="3">
         <v>45058</v>
       </c>
       <c r="E131" t="s">
@@ -5281,7 +5321,7 @@
       <c r="B132" t="s">
         <v>11</v>
       </c>
-      <c r="D132" s="1">
+      <c r="D132" s="3">
         <v>45058</v>
       </c>
       <c r="E132" t="s">
@@ -5307,7 +5347,7 @@
       <c r="B133" t="s">
         <v>11</v>
       </c>
-      <c r="D133" s="1">
+      <c r="D133" s="3">
         <v>45138</v>
       </c>
       <c r="E133" t="s">
@@ -5333,7 +5373,7 @@
       <c r="B134" t="s">
         <v>11</v>
       </c>
-      <c r="D134" s="1">
+      <c r="D134" s="3">
         <v>45138</v>
       </c>
       <c r="E134" t="s">
@@ -5359,7 +5399,7 @@
       <c r="B135" t="s">
         <v>11</v>
       </c>
-      <c r="D135" s="1">
+      <c r="D135" s="3">
         <v>45138</v>
       </c>
       <c r="E135" t="s">
@@ -5385,7 +5425,7 @@
       <c r="B136" t="s">
         <v>11</v>
       </c>
-      <c r="D136" s="1">
+      <c r="D136" s="3">
         <v>45058</v>
       </c>
       <c r="E136" t="s">
@@ -5411,7 +5451,7 @@
       <c r="B137" t="s">
         <v>11</v>
       </c>
-      <c r="D137" s="1">
+      <c r="D137" s="3">
         <v>45058</v>
       </c>
       <c r="E137" t="s">
@@ -5437,7 +5477,7 @@
       <c r="B138" t="s">
         <v>11</v>
       </c>
-      <c r="D138" s="1">
+      <c r="D138" s="3">
         <v>45145</v>
       </c>
       <c r="E138" t="s">
@@ -5463,7 +5503,7 @@
       <c r="B139" t="s">
         <v>11</v>
       </c>
-      <c r="D139" s="1">
+      <c r="D139" s="3">
         <v>45145</v>
       </c>
       <c r="E139" t="s">
@@ -5489,7 +5529,7 @@
       <c r="B140" t="s">
         <v>11</v>
       </c>
-      <c r="D140" s="1">
+      <c r="D140" s="3">
         <v>45145</v>
       </c>
       <c r="E140" t="s">
@@ -5515,7 +5555,7 @@
       <c r="B141" t="s">
         <v>11</v>
       </c>
-      <c r="D141" s="1">
+      <c r="D141" s="3">
         <v>45061</v>
       </c>
       <c r="E141" t="s">
@@ -5541,7 +5581,7 @@
       <c r="B142" t="s">
         <v>11</v>
       </c>
-      <c r="D142" s="1">
+      <c r="D142" s="3">
         <v>45061</v>
       </c>
       <c r="E142" t="s">
@@ -5567,7 +5607,7 @@
       <c r="B143" t="s">
         <v>11</v>
       </c>
-      <c r="D143" s="1">
+      <c r="D143" s="3">
         <v>45061</v>
       </c>
       <c r="E143" t="s">
@@ -5593,7 +5633,7 @@
       <c r="B144" t="s">
         <v>11</v>
       </c>
-      <c r="D144" s="1">
+      <c r="D144" s="3">
         <v>45138</v>
       </c>
       <c r="E144" t="s">
@@ -5619,7 +5659,7 @@
       <c r="B145" t="s">
         <v>11</v>
       </c>
-      <c r="D145" s="1">
+      <c r="D145" s="3">
         <v>45138</v>
       </c>
       <c r="E145" t="s">
@@ -5645,7 +5685,7 @@
       <c r="B146" t="s">
         <v>11</v>
       </c>
-      <c r="D146" s="1">
+      <c r="D146" s="3">
         <v>45138</v>
       </c>
       <c r="E146" t="s">
@@ -5671,7 +5711,7 @@
       <c r="B147" t="s">
         <v>6</v>
       </c>
-      <c r="D147" s="1">
+      <c r="D147" s="3">
         <v>45061</v>
       </c>
       <c r="E147" t="s">
@@ -5697,7 +5737,7 @@
       <c r="B148" t="s">
         <v>6</v>
       </c>
-      <c r="D148" s="1">
+      <c r="D148" s="3">
         <v>45068</v>
       </c>
       <c r="E148" t="s">
@@ -5723,7 +5763,7 @@
       <c r="B149" t="s">
         <v>6</v>
       </c>
-      <c r="D149" s="1">
+      <c r="D149" s="3">
         <v>45068</v>
       </c>
       <c r="E149" t="s">
@@ -5749,7 +5789,7 @@
       <c r="B150" t="s">
         <v>6</v>
       </c>
-      <c r="D150" s="1">
+      <c r="D150" s="3">
         <v>45152</v>
       </c>
       <c r="E150" t="s">
@@ -5775,7 +5815,7 @@
       <c r="B151" t="s">
         <v>6</v>
       </c>
-      <c r="D151" s="1">
+      <c r="D151" s="3">
         <v>45152</v>
       </c>
       <c r="E151" t="s">
@@ -5801,7 +5841,7 @@
       <c r="B152" t="s">
         <v>6</v>
       </c>
-      <c r="D152" s="1">
+      <c r="D152" s="3">
         <v>45152</v>
       </c>
       <c r="E152" t="s">
@@ -5827,7 +5867,7 @@
       <c r="B153" t="s">
         <v>11</v>
       </c>
-      <c r="D153" s="1">
+      <c r="D153" s="3">
         <v>45062</v>
       </c>
       <c r="E153" t="s">
@@ -5853,7 +5893,7 @@
       <c r="B154" t="s">
         <v>11</v>
       </c>
-      <c r="D154" s="1">
+      <c r="D154" s="3">
         <v>45062</v>
       </c>
       <c r="E154" t="s">
@@ -5879,7 +5919,7 @@
       <c r="B155" t="s">
         <v>11</v>
       </c>
-      <c r="D155" s="1">
+      <c r="D155" s="3">
         <v>45062</v>
       </c>
       <c r="E155" t="s">
@@ -5905,7 +5945,7 @@
       <c r="B156" t="s">
         <v>6</v>
       </c>
-      <c r="D156" s="1">
+      <c r="D156" s="3">
         <v>45063</v>
       </c>
       <c r="E156" t="s">
@@ -5931,7 +5971,7 @@
       <c r="B157" t="s">
         <v>6</v>
       </c>
-      <c r="D157" s="1">
+      <c r="D157" s="3">
         <v>45063</v>
       </c>
       <c r="E157" t="s">
@@ -5957,7 +5997,7 @@
       <c r="B158" t="s">
         <v>6</v>
       </c>
-      <c r="D158" s="1">
+      <c r="D158" s="3">
         <v>45063</v>
       </c>
       <c r="E158" t="s">
@@ -5983,7 +6023,7 @@
       <c r="B159" t="s">
         <v>11</v>
       </c>
-      <c r="D159" s="1">
+      <c r="D159" s="3">
         <v>45063</v>
       </c>
       <c r="E159" t="s">
@@ -6009,7 +6049,7 @@
       <c r="B160" t="s">
         <v>11</v>
       </c>
-      <c r="D160" s="1">
+      <c r="D160" s="3">
         <v>45063</v>
       </c>
       <c r="E160" t="s">
@@ -6035,7 +6075,7 @@
       <c r="B161" t="s">
         <v>11</v>
       </c>
-      <c r="D161" s="1">
+      <c r="D161" s="3">
         <v>45063</v>
       </c>
       <c r="E161" t="s">
@@ -6061,7 +6101,7 @@
       <c r="B162" t="s">
         <v>11</v>
       </c>
-      <c r="D162" s="1">
+      <c r="D162" s="3">
         <v>45138</v>
       </c>
       <c r="E162" t="s">
@@ -6087,7 +6127,7 @@
       <c r="B163" t="s">
         <v>11</v>
       </c>
-      <c r="D163" s="1">
+      <c r="D163" s="3">
         <v>45138</v>
       </c>
       <c r="E163" t="s">
@@ -6113,7 +6153,7 @@
       <c r="B164" t="s">
         <v>11</v>
       </c>
-      <c r="D164" s="1">
+      <c r="D164" s="3">
         <v>45138</v>
       </c>
       <c r="E164" t="s">
@@ -6139,7 +6179,7 @@
       <c r="B165" t="s">
         <v>11</v>
       </c>
-      <c r="D165" s="1">
+      <c r="D165" s="3">
         <v>45064</v>
       </c>
       <c r="E165" t="s">
@@ -6165,7 +6205,7 @@
       <c r="B166" t="s">
         <v>11</v>
       </c>
-      <c r="D166" s="1">
+      <c r="D166" s="3">
         <v>45064</v>
       </c>
       <c r="E166" t="s">
@@ -6191,7 +6231,7 @@
       <c r="B167" t="s">
         <v>11</v>
       </c>
-      <c r="D167" s="1">
+      <c r="D167" s="3">
         <v>45064</v>
       </c>
       <c r="E167" t="s">
@@ -6217,7 +6257,7 @@
       <c r="B168" t="s">
         <v>11</v>
       </c>
-      <c r="D168" s="1">
+      <c r="D168" s="3">
         <v>45142</v>
       </c>
       <c r="E168" t="s">
@@ -6243,7 +6283,7 @@
       <c r="B169" t="s">
         <v>11</v>
       </c>
-      <c r="D169" s="1">
+      <c r="D169" s="3">
         <v>45142</v>
       </c>
       <c r="E169" t="s">
@@ -6269,7 +6309,7 @@
       <c r="B170" t="s">
         <v>11</v>
       </c>
-      <c r="D170" s="1">
+      <c r="D170" s="3">
         <v>45142</v>
       </c>
       <c r="E170" t="s">
@@ -6295,7 +6335,7 @@
       <c r="B171" t="s">
         <v>6</v>
       </c>
-      <c r="D171" s="1">
+      <c r="D171" s="3">
         <v>45071</v>
       </c>
       <c r="E171" t="s">
@@ -6321,7 +6361,7 @@
       <c r="B172" t="s">
         <v>6</v>
       </c>
-      <c r="D172" s="1">
+      <c r="D172" s="3">
         <v>45071</v>
       </c>
       <c r="E172" t="s">
@@ -6347,7 +6387,7 @@
       <c r="B173" t="s">
         <v>6</v>
       </c>
-      <c r="D173" s="1">
+      <c r="D173" s="3">
         <v>45071</v>
       </c>
       <c r="E173" t="s">
@@ -6373,7 +6413,7 @@
       <c r="B174" t="s">
         <v>6</v>
       </c>
-      <c r="D174" s="1">
+      <c r="D174" s="3">
         <v>45141</v>
       </c>
       <c r="E174" t="s">
@@ -6399,7 +6439,7 @@
       <c r="B175" t="s">
         <v>6</v>
       </c>
-      <c r="D175" s="1">
+      <c r="D175" s="3">
         <v>45141</v>
       </c>
       <c r="E175" t="s">
@@ -6425,7 +6465,7 @@
       <c r="B176" t="s">
         <v>6</v>
       </c>
-      <c r="D176" s="1">
+      <c r="D176" s="3">
         <v>45141</v>
       </c>
       <c r="E176" t="s">
@@ -6451,7 +6491,7 @@
       <c r="B177" t="s">
         <v>11</v>
       </c>
-      <c r="D177" s="1">
+      <c r="D177" s="3">
         <v>45071</v>
       </c>
       <c r="E177" t="s">
@@ -6477,7 +6517,7 @@
       <c r="B178" t="s">
         <v>11</v>
       </c>
-      <c r="D178" s="1">
+      <c r="D178" s="3">
         <v>45071</v>
       </c>
       <c r="E178" t="s">
@@ -6503,7 +6543,7 @@
       <c r="B179" t="s">
         <v>11</v>
       </c>
-      <c r="D179" s="1">
+      <c r="D179" s="3">
         <v>45071</v>
       </c>
       <c r="E179" t="s">
@@ -6529,7 +6569,7 @@
       <c r="B180" t="s">
         <v>11</v>
       </c>
-      <c r="D180" s="1">
+      <c r="D180" s="3">
         <v>45154</v>
       </c>
       <c r="E180" t="s">
@@ -6555,7 +6595,7 @@
       <c r="B181" t="s">
         <v>11</v>
       </c>
-      <c r="D181" s="1">
+      <c r="D181" s="3">
         <v>45154</v>
       </c>
       <c r="E181" t="s">
@@ -6581,7 +6621,7 @@
       <c r="B182" t="s">
         <v>11</v>
       </c>
-      <c r="D182" s="1">
+      <c r="D182" s="3">
         <v>45154</v>
       </c>
       <c r="E182" t="s">
@@ -6607,7 +6647,7 @@
       <c r="B183" t="s">
         <v>11</v>
       </c>
-      <c r="D183" s="1">
+      <c r="D183" s="3">
         <v>45072</v>
       </c>
       <c r="E183" t="s">
@@ -6633,7 +6673,7 @@
       <c r="B184" t="s">
         <v>11</v>
       </c>
-      <c r="D184" s="1">
+      <c r="D184" s="3">
         <v>45072</v>
       </c>
       <c r="E184" t="s">
@@ -6659,7 +6699,7 @@
       <c r="B185" t="s">
         <v>11</v>
       </c>
-      <c r="D185" s="1">
+      <c r="D185" s="3">
         <v>45072</v>
       </c>
       <c r="E185" t="s">
@@ -6685,7 +6725,7 @@
       <c r="B186" t="s">
         <v>11</v>
       </c>
-      <c r="D186" s="1">
+      <c r="D186" s="3">
         <v>45078</v>
       </c>
       <c r="E186" t="s">
@@ -6711,7 +6751,7 @@
       <c r="B187" t="s">
         <v>11</v>
       </c>
-      <c r="D187" s="1">
+      <c r="D187" s="3">
         <v>45078</v>
       </c>
       <c r="E187" t="s">
@@ -6737,7 +6777,7 @@
       <c r="B188" t="s">
         <v>11</v>
       </c>
-      <c r="D188" s="1">
+      <c r="D188" s="3">
         <v>45078</v>
       </c>
       <c r="E188" t="s">
@@ -6763,7 +6803,7 @@
       <c r="B189" t="s">
         <v>6</v>
       </c>
-      <c r="D189" s="1">
+      <c r="D189" s="3">
         <v>45082</v>
       </c>
       <c r="E189" t="s">
@@ -6789,7 +6829,7 @@
       <c r="B190" t="s">
         <v>6</v>
       </c>
-      <c r="D190" s="1">
+      <c r="D190" s="3">
         <v>45082</v>
       </c>
       <c r="E190" t="s">
@@ -6815,7 +6855,7 @@
       <c r="B191" t="s">
         <v>6</v>
       </c>
-      <c r="D191" s="1">
+      <c r="D191" s="3">
         <v>45082</v>
       </c>
       <c r="E191" t="s">
@@ -6841,7 +6881,7 @@
       <c r="B192" t="s">
         <v>11</v>
       </c>
-      <c r="D192" s="1">
+      <c r="D192" s="3">
         <v>45082</v>
       </c>
       <c r="E192" t="s">
@@ -6867,7 +6907,7 @@
       <c r="B193" t="s">
         <v>11</v>
       </c>
-      <c r="D193" s="1">
+      <c r="D193" s="3">
         <v>45082</v>
       </c>
       <c r="E193" t="s">
@@ -6893,7 +6933,7 @@
       <c r="B194" t="s">
         <v>11</v>
       </c>
-      <c r="D194" s="1">
+      <c r="D194" s="3">
         <v>45089</v>
       </c>
       <c r="E194" t="s">
@@ -6919,7 +6959,7 @@
       <c r="B195" t="s">
         <v>11</v>
       </c>
-      <c r="D195" s="1">
+      <c r="D195" s="3">
         <v>45086</v>
       </c>
       <c r="E195" t="s">
@@ -6945,7 +6985,7 @@
       <c r="B196" t="s">
         <v>11</v>
       </c>
-      <c r="D196" s="1">
+      <c r="D196" s="3">
         <v>45093</v>
       </c>
       <c r="E196" t="s">
@@ -6971,7 +7011,7 @@
       <c r="B197" t="s">
         <v>11</v>
       </c>
-      <c r="D197" s="1">
+      <c r="D197" s="3">
         <v>45093</v>
       </c>
       <c r="E197" t="s">
@@ -6997,7 +7037,7 @@
       <c r="B198" t="s">
         <v>11</v>
       </c>
-      <c r="D198" s="1">
+      <c r="D198" s="3">
         <v>45084</v>
       </c>
       <c r="E198" t="s">
@@ -7023,7 +7063,7 @@
       <c r="B199" t="s">
         <v>11</v>
       </c>
-      <c r="D199" s="1">
+      <c r="D199" s="3">
         <v>45084</v>
       </c>
       <c r="E199" t="s">
@@ -7049,7 +7089,7 @@
       <c r="B200" t="s">
         <v>11</v>
       </c>
-      <c r="D200" s="1">
+      <c r="D200" s="3">
         <v>45084</v>
       </c>
       <c r="E200" t="s">
@@ -7075,7 +7115,7 @@
       <c r="B201" t="s">
         <v>11</v>
       </c>
-      <c r="D201" s="1">
+      <c r="D201" s="3">
         <v>45085</v>
       </c>
       <c r="E201" t="s">
@@ -7101,7 +7141,7 @@
       <c r="B202" t="s">
         <v>11</v>
       </c>
-      <c r="D202" s="1">
+      <c r="D202" s="3">
         <v>45085</v>
       </c>
       <c r="E202" t="s">
@@ -7127,7 +7167,7 @@
       <c r="B203" t="s">
         <v>11</v>
       </c>
-      <c r="D203" s="1">
+      <c r="D203" s="3">
         <v>45085</v>
       </c>
       <c r="E203" t="s">
@@ -7153,7 +7193,7 @@
       <c r="B204" t="s">
         <v>6</v>
       </c>
-      <c r="D204" s="1">
+      <c r="D204" s="3">
         <v>45090</v>
       </c>
       <c r="E204" t="s">
@@ -7179,7 +7219,7 @@
       <c r="B205" t="s">
         <v>6</v>
       </c>
-      <c r="D205" s="1">
+      <c r="D205" s="3">
         <v>45090</v>
       </c>
       <c r="E205" t="s">
@@ -7205,7 +7245,7 @@
       <c r="B206" t="s">
         <v>6</v>
       </c>
-      <c r="D206" s="1">
+      <c r="D206" s="3">
         <v>45090</v>
       </c>
       <c r="E206" t="s">
@@ -7231,7 +7271,7 @@
       <c r="B207" t="s">
         <v>6</v>
       </c>
-      <c r="D207" s="1">
+      <c r="D207" s="3">
         <v>45090</v>
       </c>
       <c r="E207" t="s">
@@ -7257,7 +7297,7 @@
       <c r="B208" t="s">
         <v>6</v>
       </c>
-      <c r="D208" s="1">
+      <c r="D208" s="3">
         <v>45093</v>
       </c>
       <c r="E208" s="2">
@@ -7283,7 +7323,7 @@
       <c r="B209" t="s">
         <v>6</v>
       </c>
-      <c r="D209" s="1">
+      <c r="D209" s="3">
         <v>45093</v>
       </c>
       <c r="E209" t="s">
@@ -7309,7 +7349,7 @@
       <c r="B210" t="s">
         <v>11</v>
       </c>
-      <c r="D210" s="1">
+      <c r="D210" s="3">
         <v>45091</v>
       </c>
       <c r="E210" t="s">
@@ -7335,7 +7375,7 @@
       <c r="B211" t="s">
         <v>11</v>
       </c>
-      <c r="D211" s="1">
+      <c r="D211" s="3">
         <v>45091</v>
       </c>
       <c r="E211" t="s">
@@ -7361,7 +7401,7 @@
       <c r="B212" t="s">
         <v>11</v>
       </c>
-      <c r="D212" s="1">
+      <c r="D212" s="3">
         <v>45091</v>
       </c>
       <c r="E212" t="s">
@@ -7387,7 +7427,7 @@
       <c r="B213" t="s">
         <v>6</v>
       </c>
-      <c r="D213" s="1">
+      <c r="D213" s="3">
         <v>45092</v>
       </c>
       <c r="E213" t="s">
@@ -7413,7 +7453,7 @@
       <c r="B214" t="s">
         <v>6</v>
       </c>
-      <c r="D214" s="1">
+      <c r="D214" s="3">
         <v>45097</v>
       </c>
       <c r="E214" t="s">
@@ -7439,7 +7479,7 @@
       <c r="B215" t="s">
         <v>6</v>
       </c>
-      <c r="D215" s="1" t="s">
+      <c r="D215" s="3" t="s">
         <v>296</v>
       </c>
       <c r="E215" t="s">
@@ -7465,7 +7505,7 @@
       <c r="B216" t="s">
         <v>6</v>
       </c>
-      <c r="D216" s="1">
+      <c r="D216" s="3">
         <v>45096</v>
       </c>
       <c r="E216" t="s">
@@ -7491,7 +7531,7 @@
       <c r="B217" t="s">
         <v>6</v>
       </c>
-      <c r="D217" s="1">
+      <c r="D217" s="3">
         <v>45096</v>
       </c>
       <c r="E217" t="s">
@@ -7517,7 +7557,7 @@
       <c r="B218" t="s">
         <v>11</v>
       </c>
-      <c r="D218" s="1">
+      <c r="D218" s="3">
         <v>45096</v>
       </c>
       <c r="E218" t="s">
@@ -7543,7 +7583,7 @@
       <c r="B219" t="s">
         <v>11</v>
       </c>
-      <c r="D219" s="1">
+      <c r="D219" s="3">
         <v>45096</v>
       </c>
       <c r="E219" t="s">
@@ -7569,7 +7609,7 @@
       <c r="B220" t="s">
         <v>11</v>
       </c>
-      <c r="D220" s="1">
+      <c r="D220" s="3">
         <v>45096</v>
       </c>
       <c r="E220" t="s">
@@ -7595,7 +7635,7 @@
       <c r="B221" t="s">
         <v>6</v>
       </c>
-      <c r="D221" s="1">
+      <c r="D221" s="3">
         <v>45099</v>
       </c>
       <c r="E221" t="s">
@@ -7621,7 +7661,7 @@
       <c r="B222" t="s">
         <v>6</v>
       </c>
-      <c r="D222" s="1">
+      <c r="D222" s="3">
         <v>45099</v>
       </c>
       <c r="E222" t="s">
@@ -7647,7 +7687,7 @@
       <c r="B223" t="s">
         <v>6</v>
       </c>
-      <c r="D223" s="1">
+      <c r="D223" s="3">
         <v>45099</v>
       </c>
       <c r="E223" t="s">
@@ -7673,7 +7713,7 @@
       <c r="B224" t="s">
         <v>11</v>
       </c>
-      <c r="D224" s="1">
+      <c r="D224" s="3">
         <v>45126</v>
       </c>
       <c r="E224" s="2">
@@ -7699,7 +7739,7 @@
       <c r="B225" t="s">
         <v>11</v>
       </c>
-      <c r="D225" s="1">
+      <c r="D225" s="3">
         <v>45126</v>
       </c>
       <c r="E225" s="2">
@@ -7725,7 +7765,7 @@
       <c r="B226" t="s">
         <v>11</v>
       </c>
-      <c r="D226" s="1">
+      <c r="D226" s="3">
         <v>45126</v>
       </c>
       <c r="E226" s="2">
@@ -7751,7 +7791,7 @@
       <c r="B227" t="s">
         <v>11</v>
       </c>
-      <c r="D227" s="1">
+      <c r="D227" s="3">
         <v>45128</v>
       </c>
       <c r="E227" t="s">
@@ -7777,7 +7817,7 @@
       <c r="B228" t="s">
         <v>11</v>
       </c>
-      <c r="D228" s="1">
+      <c r="D228" s="3">
         <v>45128</v>
       </c>
       <c r="E228" t="s">
@@ -7803,7 +7843,7 @@
       <c r="B229" t="s">
         <v>11</v>
       </c>
-      <c r="D229" s="1">
+      <c r="D229" s="3">
         <v>45128</v>
       </c>
       <c r="E229" t="s">
@@ -7829,7 +7869,7 @@
       <c r="B230" t="s">
         <v>11</v>
       </c>
-      <c r="D230" s="1">
+      <c r="D230" s="3">
         <v>45134</v>
       </c>
       <c r="E230" s="2">
@@ -7855,7 +7895,7 @@
       <c r="B231" t="s">
         <v>11</v>
       </c>
-      <c r="D231" s="1">
+      <c r="D231" s="3">
         <v>45134</v>
       </c>
       <c r="E231" s="2">
@@ -7881,7 +7921,7 @@
       <c r="B232" t="s">
         <v>11</v>
       </c>
-      <c r="D232" s="1">
+      <c r="D232" s="3">
         <v>45134</v>
       </c>
       <c r="E232" s="2">
@@ -7907,7 +7947,7 @@
       <c r="B233" t="s">
         <v>11</v>
       </c>
-      <c r="D233" s="1">
+      <c r="D233" s="3">
         <v>45139</v>
       </c>
       <c r="E233" t="s">
@@ -7933,7 +7973,7 @@
       <c r="B234" t="s">
         <v>11</v>
       </c>
-      <c r="D234" s="1">
+      <c r="D234" s="3">
         <v>45139</v>
       </c>
       <c r="E234" t="s">
@@ -7959,7 +7999,7 @@
       <c r="B235" t="s">
         <v>11</v>
       </c>
-      <c r="D235" s="1">
+      <c r="D235" s="3">
         <v>45139</v>
       </c>
       <c r="E235" t="s">
@@ -7985,7 +8025,7 @@
       <c r="B236" t="s">
         <v>11</v>
       </c>
-      <c r="D236" s="1">
+      <c r="D236" s="3">
         <v>45141</v>
       </c>
       <c r="E236" t="s">
@@ -8011,7 +8051,7 @@
       <c r="B237" t="s">
         <v>11</v>
       </c>
-      <c r="D237" s="1">
+      <c r="D237" s="3">
         <v>45141</v>
       </c>
       <c r="E237" t="s">
@@ -8037,7 +8077,7 @@
       <c r="B238" t="s">
         <v>11</v>
       </c>
-      <c r="D238" s="1">
+      <c r="D238" s="3">
         <v>45141</v>
       </c>
       <c r="E238" t="s">
@@ -8063,7 +8103,7 @@
       <c r="B239" t="s">
         <v>6</v>
       </c>
-      <c r="D239" s="1">
+      <c r="D239" s="3">
         <v>45145</v>
       </c>
       <c r="E239" t="s">
@@ -8089,7 +8129,7 @@
       <c r="B240" t="s">
         <v>6</v>
       </c>
-      <c r="D240" s="1">
+      <c r="D240" s="3">
         <v>45145</v>
       </c>
       <c r="E240" t="s">
@@ -8115,7 +8155,7 @@
       <c r="B241" t="s">
         <v>6</v>
       </c>
-      <c r="D241" s="1">
+      <c r="D241" s="3">
         <v>45145</v>
       </c>
       <c r="E241" t="s">
@@ -8141,7 +8181,7 @@
       <c r="B242" t="s">
         <v>6</v>
       </c>
-      <c r="D242" s="1">
+      <c r="D242" s="3">
         <v>45261</v>
       </c>
       <c r="E242" t="s">
@@ -8167,7 +8207,7 @@
       <c r="B243" t="s">
         <v>6</v>
       </c>
-      <c r="D243" s="1">
+      <c r="D243" s="3">
         <v>45261</v>
       </c>
       <c r="E243" t="s">
@@ -8193,7 +8233,7 @@
       <c r="B244" t="s">
         <v>11</v>
       </c>
-      <c r="D244" s="1">
+      <c r="D244" s="3">
         <v>45134</v>
       </c>
       <c r="E244" t="s">
@@ -8219,7 +8259,7 @@
       <c r="B245" t="s">
         <v>11</v>
       </c>
-      <c r="D245" s="1">
+      <c r="D245" s="3">
         <v>45134</v>
       </c>
       <c r="E245" t="s">
@@ -8245,7 +8285,7 @@
       <c r="B246" t="s">
         <v>11</v>
       </c>
-      <c r="D246" s="1">
+      <c r="D246" s="3">
         <v>45134</v>
       </c>
       <c r="E246" t="s">
@@ -8271,7 +8311,7 @@
       <c r="B247" t="s">
         <v>11</v>
       </c>
-      <c r="D247" s="1">
+      <c r="D247" s="3">
         <v>45120</v>
       </c>
       <c r="E247" t="s">
@@ -8297,7 +8337,7 @@
       <c r="B248" t="s">
         <v>11</v>
       </c>
-      <c r="D248" s="1">
+      <c r="D248" s="3">
         <v>45134</v>
       </c>
       <c r="E248" t="s">
@@ -8323,7 +8363,7 @@
       <c r="B249" t="s">
         <v>11</v>
       </c>
-      <c r="D249" s="1">
+      <c r="D249" s="3">
         <v>45134</v>
       </c>
       <c r="E249" t="s">
@@ -8349,7 +8389,7 @@
       <c r="B250" t="s">
         <v>11</v>
       </c>
-      <c r="D250" s="1">
+      <c r="D250" s="3">
         <v>45141</v>
       </c>
       <c r="E250" t="s">
@@ -8375,7 +8415,7 @@
       <c r="B251" t="s">
         <v>11</v>
       </c>
-      <c r="D251" s="1">
+      <c r="D251" s="3">
         <v>45141</v>
       </c>
       <c r="E251" t="s">
@@ -8401,7 +8441,7 @@
       <c r="B252" t="s">
         <v>11</v>
       </c>
-      <c r="D252" s="1">
+      <c r="D252" s="3">
         <v>45141</v>
       </c>
       <c r="E252" t="s">

</xml_diff>